<commit_message>
Update na otgovornicite po dokumenti
</commit_message>
<xml_diff>
--- a/I1/ABM-I1-DevilerablesAndRoles.xlsx
+++ b/I1/ABM-I1-DevilerablesAndRoles.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="88">
   <si>
     <t> Наименование</t>
   </si>
@@ -557,16 +557,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -574,9 +571,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -952,8 +946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -964,780 +958,807 @@
     <col min="8" max="8" width="5.28515625" customWidth="1"/>
     <col min="9" max="9" width="7.28515625" customWidth="1"/>
     <col min="10" max="10" width="7.28515625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="15.85546875" style="8" customWidth="1"/>
-    <col min="12" max="12" width="13.7109375" style="9" customWidth="1"/>
+    <col min="11" max="12" width="13.7109375" style="7" customWidth="1"/>
     <col min="13" max="13" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10"/>
-      <c r="B1" s="11" t="s">
+      <c r="A1" s="8"/>
+      <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="J1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="16" t="s">
+      <c r="K1" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="L1"/>
+      <c r="L1" s="14"/>
     </row>
     <row r="2" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="17">
+      <c r="A2" s="15">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="K2" s="23" t="s">
+      <c r="C2" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="L2"/>
+      <c r="L2" s="21"/>
     </row>
     <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="17">
+      <c r="A3" s="15">
         <v>2</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="22"/>
-      <c r="K3" s="23" t="s">
+      <c r="C3" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="L3"/>
+      <c r="L3" s="21"/>
     </row>
     <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="17">
+      <c r="A4" s="15">
         <v>3</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="I4" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="J4" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="K4" s="23" t="s">
+      <c r="C4" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="L4"/>
+      <c r="L4" s="21"/>
     </row>
     <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="17">
+      <c r="A5" s="15">
         <v>4</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="J5" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="K5" s="23" t="s">
+      <c r="C5" s="17"/>
+      <c r="D5" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="K5" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="L5"/>
+      <c r="L5" s="21"/>
     </row>
     <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="17">
+      <c r="A6" s="15">
         <v>5</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="H6" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="I6" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="J6" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="K6" s="23" t="s">
+      <c r="C6" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="J6" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="K6" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="L6"/>
+      <c r="L6" s="21"/>
     </row>
     <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="17">
+      <c r="A7" s="15">
         <v>6</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="23"/>
-      <c r="L7"/>
+      <c r="D7" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="L7" s="21"/>
     </row>
     <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="17">
-        <v>7</v>
-      </c>
-      <c r="B8" s="24" t="s">
+      <c r="A8" s="15">
+        <v>7</v>
+      </c>
+      <c r="B8" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="H8" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="I8" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="J8" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="K8" s="23"/>
-      <c r="L8"/>
+      <c r="E8" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="K8" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="L8" s="21"/>
     </row>
     <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="17">
-        <v>8</v>
-      </c>
-      <c r="B9" s="24" t="s">
+      <c r="A9" s="15">
+        <v>8</v>
+      </c>
+      <c r="B9" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="C9" s="19"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20" t="s">
+      <c r="C9" s="17"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="G9" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="H9" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="I9" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="J9" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="K9" s="23"/>
-      <c r="L9"/>
+      <c r="F9" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="I9" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="J9" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="K9" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="L9" s="21"/>
     </row>
     <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="17">
+      <c r="A10" s="15">
         <v>9</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="H10" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="I10" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="J10" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="K10" s="23" t="s">
+      <c r="D10" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="I10" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="J10" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="K10" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="L10"/>
+      <c r="L10" s="21"/>
     </row>
     <row r="11" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="17">
-        <v>10</v>
-      </c>
-      <c r="B11" s="24" t="s">
+      <c r="A11" s="15">
+        <v>10</v>
+      </c>
+      <c r="B11" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="21"/>
-      <c r="J11" s="22"/>
-      <c r="K11" s="23" t="s">
+      <c r="C11" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="L11"/>
+      <c r="L11" s="21"/>
     </row>
     <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="17">
+      <c r="A12" s="15">
         <v>11</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="G12" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="H12" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="I12" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="J12" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="K12" s="23"/>
-      <c r="L12"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="I12" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="J12" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="K12" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="L12" s="21"/>
     </row>
     <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="17">
+      <c r="A13" s="15">
         <v>12</v>
       </c>
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="G13" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="H13" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="I13" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="J13" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="K13" s="23"/>
-      <c r="L13"/>
+      <c r="D13" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="I13" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="J13" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="K13" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="L13" s="21"/>
     </row>
     <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="17">
+      <c r="A14" s="15">
         <v>13</v>
       </c>
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="19"/>
-      <c r="D14" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="G14" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="H14" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="I14" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="J14" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="K14" s="23"/>
-      <c r="L14"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="H14" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="I14" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="J14" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="K14" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="L14" s="21"/>
     </row>
     <row r="15" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="17">
+      <c r="A15" s="15">
         <v>14</v>
       </c>
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="C15" s="19"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="G15" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="H15" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="I15" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="J15" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="K15" s="23"/>
-      <c r="L15"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="G15" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="I15" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="J15" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="K15" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="L15" s="21"/>
     </row>
     <row r="16" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="17">
+      <c r="A16" s="15">
         <v>15</v>
       </c>
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="C16" s="19"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="F16" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="G16" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="H16" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="I16" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="J16" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="K16" s="23" t="s">
+      <c r="C16" s="17"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="H16" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="I16" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="J16" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="K16" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="L16"/>
+      <c r="L16" s="21"/>
     </row>
     <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="17">
+      <c r="A17" s="15">
         <v>16</v>
       </c>
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="H17" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="I17" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="J17" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="K17" s="23"/>
-      <c r="L17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="I17" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="J17" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="K17" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="L17" s="21"/>
     </row>
     <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="17">
+      <c r="A18" s="15">
         <v>17</v>
       </c>
-      <c r="B18" s="24" t="s">
+      <c r="B18" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="F18" s="20"/>
-      <c r="G18" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="H18" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="I18" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="J18" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="K18" s="23"/>
-      <c r="L18"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="18"/>
+      <c r="G18" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="I18" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="J18" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="K18" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="L18" s="21"/>
     </row>
     <row r="19" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="17">
+      <c r="A19" s="15">
         <v>18</v>
       </c>
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="19"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="J19" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="K19" s="23"/>
-      <c r="L19"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="J19" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="K19" s="21"/>
+      <c r="L19" s="21"/>
     </row>
     <row r="20" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="17">
+      <c r="A20" s="15">
         <v>19</v>
       </c>
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="19"/>
-      <c r="D20" s="20" t="s">
+      <c r="C20" s="17"/>
+      <c r="D20" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="G20" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="H20" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="I20" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="J20" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="K20" s="23" t="s">
+      <c r="E20" s="18"/>
+      <c r="F20" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="G20" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="H20" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="I20" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="J20" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="K20" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="L20"/>
+      <c r="L20" s="21"/>
     </row>
     <row r="21" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="17">
+      <c r="A21" s="15">
         <v>20</v>
       </c>
-      <c r="B21" s="24" t="s">
+      <c r="B21" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="C21" s="19"/>
-      <c r="D21" s="20" t="s">
+      <c r="C21" s="17"/>
+      <c r="D21" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="E21" s="20" t="s">
+      <c r="E21" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="F21" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="G21" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="H21" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="I21" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="J21" s="22"/>
-      <c r="K21" s="23"/>
-      <c r="L21"/>
+      <c r="F21" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="G21" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="H21" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="I21" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="J21" s="20"/>
+      <c r="K21" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="L21" s="21"/>
     </row>
     <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="17">
+      <c r="A22" s="15">
         <v>21</v>
       </c>
-      <c r="B22" s="24" t="s">
+      <c r="B22" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="C22" s="19"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="H22" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="I22" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="J22" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="K22" s="23"/>
-      <c r="L22"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="H22" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="I22" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="J22" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="K22" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="L22" s="21"/>
     </row>
     <row r="23" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="17">
+      <c r="A23" s="15">
         <v>22</v>
       </c>
-      <c r="B23" s="24" t="s">
+      <c r="B23" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="19"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="H23" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="I23" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="J23" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="K23" s="23" t="s">
+      <c r="C23" s="17"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="H23" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="I23" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="J23" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="K23" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="L23"/>
+      <c r="L23" s="21"/>
     </row>
     <row r="24" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="17">
+      <c r="A24" s="15">
         <v>23</v>
       </c>
-      <c r="B24" s="24" t="s">
+      <c r="B24" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="C24" s="19"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="H24" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="I24" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="J24" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="K24" s="23"/>
-      <c r="L24"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="H24" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="I24" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="J24" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="K24" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="L24" s="21"/>
     </row>
     <row r="25" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="17">
+      <c r="A25" s="15">
         <v>24</v>
       </c>
-      <c r="B25" s="24" t="s">
+      <c r="B25" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="19"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="H25" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="I25" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="J25" s="22" t="s">
+      <c r="C25" s="17"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="H25" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="I25" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="J25" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="K25" s="23"/>
-      <c r="L25"/>
+      <c r="K25" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="L25" s="21"/>
     </row>
     <row r="26" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="17">
+      <c r="A26" s="15">
         <v>25</v>
       </c>
-      <c r="B26" s="24" t="s">
+      <c r="B26" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="19"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="H26" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="I26" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="J26" s="22" t="s">
+      <c r="C26" s="17"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="H26" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="I26" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="J26" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="K26" s="23"/>
-      <c r="L26"/>
+      <c r="K26" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="L26" s="21"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K27"/>
@@ -1745,105 +1766,125 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K28"/>
-      <c r="L28" s="30" t="s">
+      <c r="L28" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="M28" s="31"/>
+      <c r="M28" s="29"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K29"/>
-      <c r="L29" s="25" t="s">
+      <c r="K29" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="M29" s="26" t="s">
+      <c r="L29" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="M29" s="24" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K30"/>
-      <c r="L30" s="27" t="s">
+      <c r="K30" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="M30" s="28" t="s">
+      <c r="L30" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="M30" s="26" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K31"/>
-      <c r="L31" s="27" t="s">
+      <c r="K31" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="M31" s="29" t="s">
+      <c r="L31" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="M31" s="27" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K32"/>
-      <c r="L32" s="27" t="s">
+      <c r="K32" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="M32" s="28" t="s">
+      <c r="L32" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="M32" s="26" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="33" spans="11:13" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K33"/>
-      <c r="L33" s="27" t="s">
+      <c r="K33" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="M33" s="28" t="s">
+      <c r="L33" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="M33" s="26" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="34" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K34"/>
-      <c r="L34" s="30" t="s">
+      <c r="L34" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="M34" s="31"/>
+      <c r="M34" s="29"/>
     </row>
     <row r="35" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="K35"/>
-      <c r="L35" s="25" t="s">
+      <c r="K35" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="M35" s="26" t="s">
+      <c r="L35" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="M35" s="24" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="36" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="K36"/>
-      <c r="L36" s="27" t="s">
+      <c r="K36" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="M36" s="29" t="s">
+      <c r="L36" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="M36" s="27" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="37" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="K37"/>
-      <c r="L37" s="27" t="s">
+      <c r="K37" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="M37" s="29" t="s">
+      <c r="L37" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="M37" s="27" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="38" spans="11:13" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="K38"/>
-      <c r="L38" s="27" t="s">
+      <c r="K38" s="25" t="s">
         <v>84</v>
       </c>
-      <c r="M38" s="29" t="s">
+      <c r="L38" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="M38" s="27" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="39" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="K39"/>
-      <c r="L39" s="27" t="s">
+      <c r="K39" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="M39" s="29" t="s">
+      <c r="L39" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="M39" s="27" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1872,51 +1913,39 @@
       <c r="L45"/>
     </row>
     <row r="46" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="K46" s="3"/>
       <c r="M46" s="1"/>
     </row>
     <row r="47" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="K47" s="3"/>
       <c r="M47" s="1"/>
     </row>
     <row r="48" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="K48" s="3"/>
       <c r="M48" s="1"/>
     </row>
-    <row r="49" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="K49" s="3"/>
+    <row r="49" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M49" s="1"/>
     </row>
-    <row r="50" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="K50" s="3"/>
+    <row r="50" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M50" s="2"/>
     </row>
-    <row r="51" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="K51" s="3"/>
+    <row r="51" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M51" s="2"/>
     </row>
-    <row r="52" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="K52" s="3"/>
+    <row r="52" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M52" s="1"/>
     </row>
-    <row r="53" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="K53" s="3"/>
+    <row r="53" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M53" s="1"/>
     </row>
-    <row r="54" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="K54" s="3"/>
+    <row r="54" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M54" s="1"/>
     </row>
-    <row r="55" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="K55" s="3"/>
+    <row r="55" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M55" s="1"/>
     </row>
-    <row r="56" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="K56" s="3"/>
+    <row r="56" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M56" s="1"/>
     </row>
-    <row r="57" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="K57" s="3"/>
+    <row r="57" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M57" s="1"/>
     </row>
   </sheetData>
@@ -1947,130 +1976,130 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C2" s="7">
+      <c r="C2" s="6">
         <v>1</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="6">
         <v>2</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="6">
         <v>3</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="6">
         <v>4</v>
       </c>
-      <c r="G2" s="7">
+      <c r="G2" s="6">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="5" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="4" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="4" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="5" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="4" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="6" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="3" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="7" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="8" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="G8" s="4"/>
+      <c r="G8" s="3"/>
     </row>
     <row r="9" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
     </row>
     <row r="10" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>